<commit_message>
casos de prueba actualizados
</commit_message>
<xml_diff>
--- a/casos de prueba.xlsx
+++ b/casos de prueba.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseg\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7055A355-FDF8-441B-954D-5E534508F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{63DC6B75-344F-4C6E-A7DB-25BEF92FC691}"/>
+    <workbookView minimized="1" xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Casos Normales</t>
   </si>
@@ -86,9 +85,6 @@
     <t>Sí</t>
   </si>
   <si>
-    <t>3,456,789</t>
-  </si>
-  <si>
     <t>Liquidación completa</t>
   </si>
   <si>
@@ -101,9 +97,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>1,234,567</t>
-  </si>
-  <si>
     <t>Sin auxilio transporte</t>
   </si>
   <si>
@@ -140,9 +133,6 @@
     <t>10,000,000</t>
   </si>
   <si>
-    <t>12,345,678</t>
-  </si>
-  <si>
     <t>Incluye todos los conceptos</t>
   </si>
   <si>
@@ -177,13 +167,25 @@
   </si>
   <si>
     <t>ERROR: Valor auxilio transporte excede máximo legal</t>
+  </si>
+  <si>
+    <t>2,304.000</t>
+  </si>
+  <si>
+    <t>5,537.410</t>
+  </si>
+  <si>
+    <t>4,395.869</t>
+  </si>
+  <si>
+    <t>No aplica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +210,14 @@
       <color rgb="FF404040"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -251,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -262,6 +272,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,27 +609,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681AAE22-9162-4A52-AB92-0D630D65F4CC}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.4140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.9140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="21.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -645,7 +659,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="26.4" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -659,7 +673,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -684,51 +698,51 @@
       <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="28">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="5">
         <v>180</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="28">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" s="5">
         <v>120</v>
@@ -748,14 +762,14 @@
       <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="5">
-        <v>987.654</v>
+      <c r="I5" s="6">
+        <v>901666</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="39.65">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -769,12 +783,12 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="28">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5">
         <v>200</v>
@@ -783,30 +797,30 @@
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C8" s="5">
         <v>15</v>
@@ -815,10 +829,10 @@
         <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>15</v>
@@ -826,25 +840,25 @@
       <c r="H8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="5">
-        <v>345.678</v>
+      <c r="I8" s="6">
+        <v>133842</v>
       </c>
       <c r="J8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="42">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="5">
         <v>365</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>15</v>
@@ -858,14 +872,15 @@
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>34</v>
+      <c r="I9" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="26.4">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -879,12 +894,12 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="39.65" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5">
         <v>30</v>
@@ -905,13 +920,13 @@
         <v>15</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="39.65" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
@@ -935,15 +950,15 @@
         <v>15</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="39.65" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -953,22 +968,22 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="42">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5">
         <v>180</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
@@ -983,11 +998,11 @@
         <v>15</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.5">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -996,7 +1011,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.5">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -1005,7 +1020,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="14.5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -1016,5 +1031,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>